<commit_message>
Extended tests for GT4500 due to lack of minimum coverage
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Levi\BME\Szoftvertechnológia\Labor\se-lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A24F00-AEEE-4310-B265-33F1DCE74048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC7985C-9058-4703-8223-EEB80EB9DBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1F8C1DD-FF32-49EA-8F20-D471A09EF64C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Tesztesetek</t>
   </si>
@@ -74,9 +74,6 @@
     <t>A GT4500 megpróbál a másik tárolóból lőni, ha a sorban következő üres</t>
   </si>
   <si>
-    <t>Az egyik tároló tartalmaz 2 torpedót, a másik üres</t>
-  </si>
-  <si>
     <t>3. teszteset</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>4. teszteset</t>
   </si>
   <si>
-    <t>A GT4500 tud egyszerre tüzelni mindkét tárolóból</t>
-  </si>
-  <si>
     <t>Mindkét tároló tartalmaz legalább 1 torpedót</t>
   </si>
   <si>
@@ -105,6 +99,30 @@
   </si>
   <si>
     <t>A második parancs eredeménye SUCCESS, a harmadik parancs eredménye FAIL</t>
+  </si>
+  <si>
+    <t>A második és a harmadik, valamint az ötödik és hatodik parancs eredménye SUCCESS</t>
+  </si>
+  <si>
+    <t>Az egyik tároló tartalmaz 2 torpedót, a másik üres (mindkét tárolóval tesztelve)</t>
+  </si>
+  <si>
+    <t>A GT4500 tud egyszerre tüzelni mindkét tárolóból, ha az egyik üres, akkor a másikból tüzel, ha mindkettő üres, akkor nem tüzel</t>
+  </si>
+  <si>
+    <t>5. teszteset</t>
+  </si>
+  <si>
+    <t>A GT4500 csak a SINGLE és ALL tüzelési módokat ismeri</t>
+  </si>
+  <si>
+    <t>Hibás tüzelési módot adunk meg a GT4500-nak (pl. RANDOM)</t>
+  </si>
+  <si>
+    <t>A második parancs eredménye Unknown firing mode: 'RANDOM'</t>
+  </si>
+  <si>
+    <t>Van egy GT4500 hajó</t>
   </si>
 </sst>
 </file>
@@ -151,14 +169,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,207 +514,226 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591C306A-B0FA-4845-A592-0CB338CB9483}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="42.85546875" customWidth="1"/>
+    <col min="1" max="2" width="120.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A7:B7"/>

</xml_diff>